<commit_message>
add spin v2 xlsx
</commit_message>
<xml_diff>
--- a/xls/spin_the_movie.xlsx
+++ b/xls/spin_the_movie.xlsx
@@ -34,7 +34,7 @@
     <t>row</t>
   </si>
   <si>
-    <t>MT mem RD BW test, dura= 3.012064, GB/sec= 18.425286</t>
+    <t>MT mem RD BW test, dura= 3.012559, GB/sec= 18.216385</t>
   </si>
   <si>
     <t>Based on non-idle sched_switch ftrace event. 100% means 1 cpu is busy, 400% means 4 cpus busy, etc.; See chart: %busy system; chart_tag: PCT_BUSY_BY_SYSTEM</t>
@@ -562,13 +562,13 @@
     <t>uop_port_7/nsec core1</t>
   </si>
   <si>
-    <t>MT L3 RD BW test, dura= 3.000007, GB/sec= 65.731373</t>
-  </si>
-  <si>
-    <t>MT L2 RD BW test, dura= 3.000002, GB/sec= 135.597754</t>
-  </si>
-  <si>
-    <t>MT spin test, dura= 3.000000, Gops/sec= 3.854128</t>
+    <t>MT L3 RD BW test, dura= 3.000009, GB/sec= 65.738517</t>
+  </si>
+  <si>
+    <t>MT L2 RD BW test, dura= 3.000003, GB/sec= 133.187461</t>
+  </si>
+  <si>
+    <t>MT spin test, dura= 3.000000, Gops/sec= 3.857277</t>
   </si>
 </sst>
 </file>
@@ -1915,82 +1915,82 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>1042.097952</v>
+        <v>828.367259</v>
       </c>
       <c r="E5">
-        <v>1045.104516</v>
+        <v>831.374318</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>399.8</v>
+        <v>400</v>
       </c>
       <c r="H5">
-        <v>47.3</v>
+        <v>49.8</v>
       </c>
       <c r="I5">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="J5">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="K5">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="L5">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>18.2</v>
       </c>
       <c r="N5">
-        <v>10.3</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>14.7</v>
+        <v>13.9</v>
       </c>
       <c r="Q5">
         <v>2</v>
       </c>
       <c r="R5">
-        <v>18457.7</v>
+        <v>18242.7</v>
       </c>
       <c r="S5">
-        <v>18550</v>
+        <v>18327.7</v>
       </c>
       <c r="T5">
-        <v>92.2</v>
+        <v>85</v>
       </c>
       <c r="U5">
-        <v>73.2</v>
+        <v>72.3</v>
       </c>
       <c r="V5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="W5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="X5">
-        <v>54.5</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="Y5">
-        <v>54.2</v>
+        <v>63.9</v>
       </c>
       <c r="Z5">
-        <v>10.2</v>
+        <v>6.6</v>
       </c>
       <c r="AA5">
-        <v>10.1</v>
+        <v>6.6</v>
       </c>
       <c r="AB5">
-        <v>27.2</v>
+        <v>20.8</v>
       </c>
       <c r="AC5">
-        <v>26.9</v>
+        <v>20.8</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -1999,118 +1999,118 @@
         <v>0</v>
       </c>
       <c r="AF5">
-        <v>15.5</v>
+        <v>11.2</v>
       </c>
       <c r="AG5">
-        <v>15.1</v>
+        <v>11.1</v>
       </c>
       <c r="AH5">
-        <v>6.4</v>
+        <v>3.8</v>
       </c>
       <c r="AI5">
-        <v>6.3</v>
+        <v>3.8</v>
       </c>
       <c r="AJ5">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="AK5">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AL5">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="AM5">
-        <v>3.3</v>
+        <v>2.3</v>
       </c>
       <c r="AN5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="AO5">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="AP5">
         <v>0.02</v>
       </c>
       <c r="AQ5">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="AR5">
-        <v>0.59</v>
+        <v>0.35</v>
       </c>
       <c r="AS5">
-        <v>0.58</v>
+        <v>0.35</v>
       </c>
       <c r="AT5">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="AU5">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="AV5">
-        <v>82.09999999999999</v>
+        <v>88.2</v>
       </c>
       <c r="AW5">
-        <v>82.09999999999999</v>
+        <v>87.7</v>
       </c>
       <c r="AX5">
-        <v>82</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="AY5">
-        <v>82</v>
+        <v>88.09999999999999</v>
       </c>
       <c r="AZ5">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="BA5">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="BB5">
-        <v>0.65</v>
+        <v>0.42</v>
       </c>
       <c r="BC5">
-        <v>0.65</v>
+        <v>0.43</v>
       </c>
       <c r="BD5">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="BE5">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="BF5">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="BG5">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="BH5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="BI5">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="BJ5">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="BK5">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="BL5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="BM5">
         <v>0.01</v>
       </c>
       <c r="BN5">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="BO5">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="BP5">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="BQ5">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="BR5">
         <v>0</v>
@@ -2119,49 +2119,49 @@
         <v>0</v>
       </c>
       <c r="BT5">
-        <v>0.25</v>
+        <v>0.16</v>
       </c>
       <c r="BU5">
-        <v>0.25</v>
+        <v>0.16</v>
       </c>
       <c r="BV5">
-        <v>0.26</v>
+        <v>0.17</v>
       </c>
       <c r="BW5">
-        <v>0.26</v>
+        <v>0.17</v>
       </c>
       <c r="BX5">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="BY5">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="BZ5">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="CA5">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="CB5">
         <v>0.01</v>
       </c>
       <c r="CC5">
+        <v>0.02</v>
+      </c>
+      <c r="CD5">
+        <v>0.17</v>
+      </c>
+      <c r="CE5">
+        <v>0.17</v>
+      </c>
+      <c r="CF5">
+        <v>0.3</v>
+      </c>
+      <c r="CG5">
+        <v>0.3</v>
+      </c>
+      <c r="CH5">
         <v>0.01</v>
-      </c>
-      <c r="CD5">
-        <v>0.26</v>
-      </c>
-      <c r="CE5">
-        <v>0.26</v>
-      </c>
-      <c r="CF5">
-        <v>0.45</v>
-      </c>
-      <c r="CG5">
-        <v>0.45</v>
-      </c>
-      <c r="CH5">
-        <v>0</v>
       </c>
       <c r="CI5">
         <v>0.01</v>
@@ -2178,10 +2178,10 @@
         <v>182</v>
       </c>
       <c r="D6">
-        <v>1045.110401</v>
+        <v>831.380709</v>
       </c>
       <c r="E6">
-        <v>1048.104908</v>
+        <v>834.375218</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -2190,7 +2190,7 @@
         <v>400</v>
       </c>
       <c r="H6">
-        <v>54.9</v>
+        <v>56.8</v>
       </c>
       <c r="I6">
         <v>2.6</v>
@@ -2205,7 +2205,7 @@
         <v>2.6</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>22.6</v>
       </c>
       <c r="N6">
         <v>13</v>
@@ -2220,16 +2220,16 @@
         <v>0.5</v>
       </c>
       <c r="R6">
-        <v>518.9</v>
+        <v>519.1</v>
       </c>
       <c r="S6">
         <v>524.9</v>
       </c>
       <c r="T6">
-        <v>5.9</v>
+        <v>5.8</v>
       </c>
       <c r="U6">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -2238,10 +2238,10 @@
         <v>0</v>
       </c>
       <c r="X6">
-        <v>29.4</v>
+        <v>29.3</v>
       </c>
       <c r="Y6">
-        <v>29.4</v>
+        <v>29.2</v>
       </c>
       <c r="Z6">
         <v>19.3</v>
@@ -2250,10 +2250,10 @@
         <v>19.3</v>
       </c>
       <c r="AB6">
-        <v>43.3</v>
+        <v>43.4</v>
       </c>
       <c r="AC6">
-        <v>43.3</v>
+        <v>43.1</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -2262,10 +2262,10 @@
         <v>0</v>
       </c>
       <c r="AF6">
-        <v>25.7</v>
+        <v>25.8</v>
       </c>
       <c r="AG6">
-        <v>25.6</v>
+        <v>25.5</v>
       </c>
       <c r="AH6">
         <v>12.8</v>
@@ -2274,7 +2274,7 @@
         <v>12.8</v>
       </c>
       <c r="AJ6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AK6">
         <v>0.2</v>
@@ -2283,7 +2283,7 @@
         <v>0.2</v>
       </c>
       <c r="AM6">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AN6">
         <v>0.1</v>
@@ -2295,10 +2295,10 @@
         <v>0.02</v>
       </c>
       <c r="AQ6">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="AR6">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="AS6">
         <v>1.19</v>
@@ -2310,28 +2310,28 @@
         <v>0.01</v>
       </c>
       <c r="AV6">
-        <v>67</v>
+        <v>66.8</v>
       </c>
       <c r="AW6">
-        <v>67.09999999999999</v>
+        <v>66.7</v>
       </c>
       <c r="AX6">
         <v>66.3</v>
       </c>
       <c r="AY6">
-        <v>66.3</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="AZ6">
         <v>1.1</v>
       </c>
       <c r="BA6">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="BB6">
         <v>1.22</v>
       </c>
       <c r="BC6">
-        <v>1.22</v>
+        <v>1.23</v>
       </c>
       <c r="BD6">
         <v>0.19</v>
@@ -2367,7 +2367,7 @@
         <v>0.2</v>
       </c>
       <c r="BO6">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="BP6">
         <v>0.34</v>
@@ -2403,19 +2403,19 @@
         <v>0.27</v>
       </c>
       <c r="CA6">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
       <c r="CB6">
+        <v>0.02</v>
+      </c>
+      <c r="CC6">
         <v>0.01</v>
       </c>
-      <c r="CC6">
-        <v>0.02</v>
-      </c>
       <c r="CD6">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="CE6">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="CF6">
         <v>0.88</v>
@@ -2441,19 +2441,19 @@
         <v>183</v>
       </c>
       <c r="D7">
-        <v>1048.11264</v>
+        <v>834.388636</v>
       </c>
       <c r="E7">
-        <v>1051.107142</v>
+        <v>837.383139</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>400</v>
+        <v>399.7</v>
       </c>
       <c r="H7">
-        <v>59.6</v>
+        <v>61.5</v>
       </c>
       <c r="I7">
         <v>2.6</v>
@@ -2468,7 +2468,7 @@
         <v>2.6</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>23.1</v>
       </c>
       <c r="N7">
         <v>13.5</v>
@@ -2477,19 +2477,19 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>16.9</v>
+        <v>16.7</v>
       </c>
       <c r="Q7">
         <v>0.5</v>
       </c>
       <c r="R7">
-        <v>504.5</v>
+        <v>493.5</v>
       </c>
       <c r="S7">
-        <v>509.4</v>
+        <v>498.6</v>
       </c>
       <c r="T7">
-        <v>4.9</v>
+        <v>5.1</v>
       </c>
       <c r="U7">
         <v>0.1</v>
@@ -2501,22 +2501,22 @@
         <v>0</v>
       </c>
       <c r="X7">
+        <v>0.2</v>
+      </c>
+      <c r="Y7">
         <v>0.1</v>
       </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
       <c r="Z7">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="AA7">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AB7">
-        <v>39.5</v>
+        <v>41.2</v>
       </c>
       <c r="AC7">
-        <v>40.5</v>
+        <v>40.4</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -2525,16 +2525,16 @@
         <v>0</v>
       </c>
       <c r="AF7">
-        <v>17.3</v>
+        <v>17.6</v>
       </c>
       <c r="AG7">
-        <v>17.3</v>
+        <v>17.2</v>
       </c>
       <c r="AH7">
-        <v>26.4</v>
+        <v>25.8</v>
       </c>
       <c r="AI7">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="AJ7">
         <v>0.1</v>
@@ -2543,13 +2543,13 @@
         <v>0.1</v>
       </c>
       <c r="AL7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AM7">
         <v>0.3</v>
       </c>
       <c r="AN7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AO7">
         <v>0.3</v>
@@ -2561,64 +2561,64 @@
         <v>0.1</v>
       </c>
       <c r="AR7">
-        <v>2.42</v>
+        <v>2.37</v>
       </c>
       <c r="AS7">
-        <v>2.42</v>
+        <v>2.38</v>
       </c>
       <c r="AT7">
         <v>0.01</v>
       </c>
       <c r="AU7">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="AV7">
-        <v>30.5</v>
+        <v>32</v>
       </c>
       <c r="AW7">
-        <v>30.4</v>
+        <v>31.6</v>
       </c>
       <c r="AX7">
-        <v>33</v>
+        <v>34.2</v>
       </c>
       <c r="AY7">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AZ7">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="BA7">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="BB7">
-        <v>2.52</v>
+        <v>2.47</v>
       </c>
       <c r="BC7">
-        <v>2.52</v>
+        <v>2.5</v>
       </c>
       <c r="BD7">
+        <v>0.38</v>
+      </c>
+      <c r="BE7">
+        <v>0.38</v>
+      </c>
+      <c r="BF7">
         <v>0.39</v>
       </c>
-      <c r="BE7">
+      <c r="BG7">
         <v>0.39</v>
       </c>
-      <c r="BF7">
-        <v>0.4</v>
-      </c>
-      <c r="BG7">
-        <v>0.4</v>
-      </c>
       <c r="BH7">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="BI7">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="BJ7">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="BK7">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="BL7">
         <v>0.01</v>
@@ -2627,16 +2627,16 @@
         <v>0.01</v>
       </c>
       <c r="BN7">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="BO7">
         <v>0.4</v>
       </c>
       <c r="BP7">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="BQ7">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="BR7">
         <v>0.01</v>
@@ -2645,28 +2645,28 @@
         <v>0.01</v>
       </c>
       <c r="BT7">
+        <v>0.98</v>
+      </c>
+      <c r="BU7">
+        <v>0.99</v>
+      </c>
+      <c r="BV7">
+        <v>1</v>
+      </c>
+      <c r="BW7">
         <v>1.01</v>
       </c>
-      <c r="BU7">
-        <v>1.01</v>
-      </c>
-      <c r="BV7">
-        <v>1.02</v>
-      </c>
-      <c r="BW7">
-        <v>1.03</v>
-      </c>
       <c r="BX7">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="BY7">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="BZ7">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="CA7">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="CB7">
         <v>0.03</v>
@@ -2675,22 +2675,22 @@
         <v>0.03</v>
       </c>
       <c r="CD7">
-        <v>1.04</v>
+        <v>1.01</v>
       </c>
       <c r="CE7">
-        <v>1.04</v>
+        <v>1.02</v>
       </c>
       <c r="CF7">
-        <v>1.68</v>
+        <v>1.65</v>
       </c>
       <c r="CG7">
-        <v>1.68</v>
+        <v>1.66</v>
       </c>
       <c r="CH7">
         <v>0.01</v>
       </c>
       <c r="CI7">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="8" spans="1:87">
@@ -2704,10 +2704,10 @@
         <v>184</v>
       </c>
       <c r="D8">
-        <v>1051.114764</v>
+        <v>837.392574</v>
       </c>
       <c r="E8">
-        <v>1054.109264</v>
+        <v>840.387074</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -2716,7 +2716,7 @@
         <v>400</v>
       </c>
       <c r="H8">
-        <v>62.9</v>
+        <v>65.5</v>
       </c>
       <c r="I8">
         <v>2.6</v>
@@ -2731,10 +2731,10 @@
         <v>2.6</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>23.1</v>
       </c>
       <c r="N8">
-        <v>13.3</v>
+        <v>13.1</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -2746,13 +2746,13 @@
         <v>0.5</v>
       </c>
       <c r="R8">
-        <v>499.6</v>
+        <v>482.8</v>
       </c>
       <c r="S8">
-        <v>504.6</v>
+        <v>487.3</v>
       </c>
       <c r="T8">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="U8">
         <v>0.1</v>
@@ -2776,10 +2776,10 @@
         <v>0</v>
       </c>
       <c r="AB8">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AC8">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -2788,16 +2788,16 @@
         <v>0</v>
       </c>
       <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
         <v>0.1</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0.1</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
       </c>
       <c r="AJ8">
         <v>0</v>
@@ -2809,7 +2809,7 @@
         <v>0.1</v>
       </c>
       <c r="AM8">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AN8">
         <v>0.1</v>
@@ -2818,16 +2818,16 @@
         <v>0.1</v>
       </c>
       <c r="AP8">
-        <v>2.85</v>
+        <v>2.87</v>
       </c>
       <c r="AQ8">
-        <v>2.85</v>
+        <v>2.84</v>
       </c>
       <c r="AR8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AS8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AT8">
         <v>0.21</v>
@@ -2836,31 +2836,31 @@
         <v>0.21</v>
       </c>
       <c r="AV8">
-        <v>11.7</v>
+        <v>11.4</v>
       </c>
       <c r="AW8">
-        <v>11.6</v>
+        <v>11.4</v>
       </c>
       <c r="AX8">
-        <v>8.6</v>
+        <v>8</v>
       </c>
       <c r="AY8">
-        <v>8.4</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="AZ8">
+        <v>0.7</v>
+      </c>
+      <c r="BA8">
         <v>0.8</v>
       </c>
-      <c r="BA8">
-        <v>0.9</v>
-      </c>
       <c r="BB8">
-        <v>3.3</v>
+        <v>3.31</v>
       </c>
       <c r="BC8">
-        <v>3.3</v>
+        <v>3.31</v>
       </c>
       <c r="BD8">
-        <v>0.55</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="BE8">
         <v>0.55</v>
@@ -2893,7 +2893,7 @@
         <v>0.63</v>
       </c>
       <c r="BO8">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="BP8">
         <v>0.75</v>
@@ -2914,7 +2914,7 @@
         <v>1.43</v>
       </c>
       <c r="BV8">
-        <v>1.52</v>
+        <v>1.53</v>
       </c>
       <c r="BW8">
         <v>1.52</v>
@@ -2938,16 +2938,16 @@
         <v>0.64</v>
       </c>
       <c r="CD8">
-        <v>1.62</v>
+        <v>1.63</v>
       </c>
       <c r="CE8">
-        <v>1.62</v>
+        <v>1.61</v>
       </c>
       <c r="CF8">
+        <v>1.94</v>
+      </c>
+      <c r="CG8">
         <v>1.93</v>
-      </c>
-      <c r="CG8">
-        <v>1.94</v>
       </c>
       <c r="CH8">
         <v>0.33</v>

</xml_diff>